<commit_message>
x1469 Humans have been renamed "Homo sapiens (Human)"
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/block_reg.xlsx
+++ b/src/test/resources/testdata/block_reg.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dr6/Code/stan/core/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB46293A-7C58-F94C-8B70-F1D2926D986D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59177633-906C-AB42-8FD2-CE6F6D5BCB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="760" windowWidth="27640" windowHeight="15900" activeTab="2" xr2:uid="{5C25E200-6C46-9D45-98E6-7DE84B4E9124}"/>
   </bookViews>
@@ -114,9 +114,6 @@
     <t>Adult</t>
   </si>
   <si>
-    <t>Human</t>
-  </si>
-  <si>
     <t>19/0067</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>Organoid</t>
+  </si>
+  <si>
+    <t>Homo sapiens (Human)</t>
   </si>
 </sst>
 </file>
@@ -568,7 +568,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,13 +627,13 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J2" t="s">
         <v>11</v>
@@ -680,22 +680,22 @@
         <v>44705</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
         <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -707,42 +707,42 @@
         <v>19</v>
       </c>
       <c r="O3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" t="s">
         <v>28</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>29</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
         <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
       </c>
       <c r="E4">
         <v>44705</v>
       </c>
       <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>34</v>
-      </c>
-      <c r="K4" t="s">
-        <v>35</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -754,21 +754,21 @@
         <v>19</v>
       </c>
       <c r="O4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" t="s">
         <v>28</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>29</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
@@ -777,22 +777,22 @@
         <v>44706</v>
       </c>
       <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="G5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" t="s">
         <v>25</v>
       </c>
-      <c r="I5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" t="s">
-        <v>26</v>
-      </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L5">
         <v>2</v>
@@ -804,16 +804,16 @@
         <v>21</v>
       </c>
       <c r="O5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" t="s">
         <v>40</v>
-      </c>
-      <c r="R5" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>